<commit_message>
fix for constraint so that bed is assigned to everyone with treatment
</commit_message>
<xml_diff>
--- a/game3/Challenge3_Day1Submission_jaimie.xlsx
+++ b/game3/Challenge3_Day1Submission_jaimie.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jaimie\Desktop\gitRepos\HackTheMachine\game3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leeb\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A8D1CC7-3D86-4392-9EB6-9C329F19B58B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{36F5FBB2-190D-4257-9FB0-82B96F9E133F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Challenge3_Day1Submission_jaimi" sheetId="1" r:id="rId1"/>
@@ -20,37 +20,37 @@
     <definedName name="solver_adj" localSheetId="0" hidden="1">Challenge3_Day1Submission_jaimi!$D$2:$D$21,Challenge3_Day1Submission_jaimi!$F$2:$F$21,Challenge3_Day1Submission_jaimi!$H$2:$H$21,Challenge3_Day1Submission_jaimi!$J$2:$J$21,Challenge3_Day1Submission_jaimi!$L$2:$L$21,Challenge3_Day1Submission_jaimi!$N$2:$N$21,Challenge3_Day1Submission_jaimi!$P$2:$P$21,Challenge3_Day1Submission_jaimi!$R$2:$R$21</definedName>
     <definedName name="solver_cvg" localSheetId="0" hidden="1">0.0001</definedName>
     <definedName name="solver_drv" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_eng" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_eng" localSheetId="0" hidden="1">3</definedName>
     <definedName name="solver_est" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_itr" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_lhs1" localSheetId="0" hidden="1">Challenge3_Day1Submission_jaimi!$D$22</definedName>
-    <definedName name="solver_lhs10" localSheetId="0" hidden="1">Challenge3_Day1Submission_jaimi!$J$22</definedName>
-    <definedName name="solver_lhs11" localSheetId="0" hidden="1">Challenge3_Day1Submission_jaimi!$J$2:$J$21</definedName>
+    <definedName name="solver_lhs10" localSheetId="0" hidden="1">Challenge3_Day1Submission_jaimi!$H$2:$H$21</definedName>
+    <definedName name="solver_lhs11" localSheetId="0" hidden="1">Challenge3_Day1Submission_jaimi!$J$22</definedName>
     <definedName name="solver_lhs12" localSheetId="0" hidden="1">Challenge3_Day1Submission_jaimi!$J$2:$J$21</definedName>
-    <definedName name="solver_lhs13" localSheetId="0" hidden="1">Challenge3_Day1Submission_jaimi!$L$22</definedName>
-    <definedName name="solver_lhs14" localSheetId="0" hidden="1">Challenge3_Day1Submission_jaimi!$L$2:$L$21</definedName>
+    <definedName name="solver_lhs13" localSheetId="0" hidden="1">Challenge3_Day1Submission_jaimi!$J$2:$J$21</definedName>
+    <definedName name="solver_lhs14" localSheetId="0" hidden="1">Challenge3_Day1Submission_jaimi!$L$22</definedName>
     <definedName name="solver_lhs15" localSheetId="0" hidden="1">Challenge3_Day1Submission_jaimi!$L$2:$L$21</definedName>
-    <definedName name="solver_lhs16" localSheetId="0" hidden="1">Challenge3_Day1Submission_jaimi!$N$22</definedName>
-    <definedName name="solver_lhs17" localSheetId="0" hidden="1">Challenge3_Day1Submission_jaimi!$N$2:$N$21</definedName>
+    <definedName name="solver_lhs16" localSheetId="0" hidden="1">Challenge3_Day1Submission_jaimi!$L$2:$L$21</definedName>
+    <definedName name="solver_lhs17" localSheetId="0" hidden="1">Challenge3_Day1Submission_jaimi!$N$22</definedName>
     <definedName name="solver_lhs18" localSheetId="0" hidden="1">Challenge3_Day1Submission_jaimi!$N$2:$N$21</definedName>
-    <definedName name="solver_lhs19" localSheetId="0" hidden="1">Challenge3_Day1Submission_jaimi!$P$22</definedName>
+    <definedName name="solver_lhs19" localSheetId="0" hidden="1">Challenge3_Day1Submission_jaimi!$N$2:$N$21</definedName>
     <definedName name="solver_lhs2" localSheetId="0" hidden="1">Challenge3_Day1Submission_jaimi!$D$2:$D$21</definedName>
-    <definedName name="solver_lhs20" localSheetId="0" hidden="1">Challenge3_Day1Submission_jaimi!$P$2:$P$21</definedName>
+    <definedName name="solver_lhs20" localSheetId="0" hidden="1">Challenge3_Day1Submission_jaimi!$P$22</definedName>
     <definedName name="solver_lhs21" localSheetId="0" hidden="1">Challenge3_Day1Submission_jaimi!$P$2:$P$21</definedName>
-    <definedName name="solver_lhs22" localSheetId="0" hidden="1">Challenge3_Day1Submission_jaimi!$R$22</definedName>
-    <definedName name="solver_lhs23" localSheetId="0" hidden="1">Challenge3_Day1Submission_jaimi!$R$2:$R$21</definedName>
+    <definedName name="solver_lhs22" localSheetId="0" hidden="1">Challenge3_Day1Submission_jaimi!$P$2:$P$21</definedName>
+    <definedName name="solver_lhs23" localSheetId="0" hidden="1">Challenge3_Day1Submission_jaimi!$R$22</definedName>
     <definedName name="solver_lhs24" localSheetId="0" hidden="1">Challenge3_Day1Submission_jaimi!$R$2:$R$21</definedName>
-    <definedName name="solver_lhs25" localSheetId="0" hidden="1">Challenge3_Day1Submission_jaimi!$S$2:$S$21</definedName>
+    <definedName name="solver_lhs25" localSheetId="0" hidden="1">Challenge3_Day1Submission_jaimi!$R$2:$R$21</definedName>
     <definedName name="solver_lhs26" localSheetId="0" hidden="1">Challenge3_Day1Submission_jaimi!$S$2:$S$21</definedName>
     <definedName name="solver_lhs27" localSheetId="0" hidden="1">Challenge3_Day1Submission_jaimi!$S$2:$S$21</definedName>
     <definedName name="solver_lhs28" localSheetId="0" hidden="1">Challenge3_Day1Submission_jaimi!$S$2:$S$21</definedName>
     <definedName name="solver_lhs29" localSheetId="0" hidden="1">Challenge3_Day1Submission_jaimi!$S$2:$S$21</definedName>
     <definedName name="solver_lhs3" localSheetId="0" hidden="1">Challenge3_Day1Submission_jaimi!$D$2:$D$21</definedName>
-    <definedName name="solver_lhs4" localSheetId="0" hidden="1">Challenge3_Day1Submission_jaimi!$F$22</definedName>
-    <definedName name="solver_lhs5" localSheetId="0" hidden="1">Challenge3_Day1Submission_jaimi!$F$2:$F$21</definedName>
+    <definedName name="solver_lhs4" localSheetId="0" hidden="1">Challenge3_Day1Submission_jaimi!$D$2:$D$21</definedName>
+    <definedName name="solver_lhs5" localSheetId="0" hidden="1">Challenge3_Day1Submission_jaimi!$F$22</definedName>
     <definedName name="solver_lhs6" localSheetId="0" hidden="1">Challenge3_Day1Submission_jaimi!$F$2:$F$21</definedName>
-    <definedName name="solver_lhs7" localSheetId="0" hidden="1">Challenge3_Day1Submission_jaimi!$H$22</definedName>
-    <definedName name="solver_lhs8" localSheetId="0" hidden="1">Challenge3_Day1Submission_jaimi!$H$2:$H$21</definedName>
+    <definedName name="solver_lhs7" localSheetId="0" hidden="1">Challenge3_Day1Submission_jaimi!$F$2:$F$21</definedName>
+    <definedName name="solver_lhs8" localSheetId="0" hidden="1">Challenge3_Day1Submission_jaimi!$H$22</definedName>
     <definedName name="solver_lhs9" localSheetId="0" hidden="1">Challenge3_Day1Submission_jaimi!$H$2:$H$21</definedName>
     <definedName name="solver_mip" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_mni" localSheetId="0" hidden="1">30</definedName>
@@ -58,69 +58,69 @@
     <definedName name="solver_msl" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_neg" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_nod" localSheetId="0" hidden="1">2147483647</definedName>
-    <definedName name="solver_num" localSheetId="0" hidden="1">25</definedName>
+    <definedName name="solver_num" localSheetId="0" hidden="1">26</definedName>
     <definedName name="solver_nwt" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_opt" localSheetId="0" hidden="1">Challenge3_Day1Submission_jaimi!$V$24</definedName>
+    <definedName name="solver_opt" localSheetId="0" hidden="1">Challenge3_Day1Submission_jaimi!$W$24</definedName>
     <definedName name="solver_pre" localSheetId="0" hidden="1">0.000001</definedName>
     <definedName name="solver_rbv" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rel1" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_rel10" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rel10" localSheetId="0" hidden="1">4</definedName>
     <definedName name="solver_rel11" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_rel12" localSheetId="0" hidden="1">4</definedName>
-    <definedName name="solver_rel13" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rel12" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rel13" localSheetId="0" hidden="1">4</definedName>
     <definedName name="solver_rel14" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_rel15" localSheetId="0" hidden="1">4</definedName>
-    <definedName name="solver_rel16" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rel15" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rel16" localSheetId="0" hidden="1">4</definedName>
     <definedName name="solver_rel17" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_rel18" localSheetId="0" hidden="1">4</definedName>
-    <definedName name="solver_rel19" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rel18" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rel19" localSheetId="0" hidden="1">4</definedName>
     <definedName name="solver_rel2" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rel20" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_rel21" localSheetId="0" hidden="1">4</definedName>
-    <definedName name="solver_rel22" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rel21" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rel22" localSheetId="0" hidden="1">4</definedName>
     <definedName name="solver_rel23" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_rel24" localSheetId="0" hidden="1">4</definedName>
-    <definedName name="solver_rel25" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rel24" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rel25" localSheetId="0" hidden="1">4</definedName>
     <definedName name="solver_rel26" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rel27" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rel28" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rel29" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rel3" localSheetId="0" hidden="1">4</definedName>
-    <definedName name="solver_rel4" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rel4" localSheetId="0" hidden="1">3</definedName>
     <definedName name="solver_rel5" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_rel6" localSheetId="0" hidden="1">4</definedName>
-    <definedName name="solver_rel7" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rel6" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rel7" localSheetId="0" hidden="1">4</definedName>
     <definedName name="solver_rel8" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_rel9" localSheetId="0" hidden="1">4</definedName>
+    <definedName name="solver_rel9" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rhs1" localSheetId="0" hidden="1">Challenge3_Day1Submission_jaimi!$B$2</definedName>
-    <definedName name="solver_rhs10" localSheetId="0" hidden="1">Challenge3_Day1Submission_jaimi!$B$5</definedName>
-    <definedName name="solver_rhs11" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_rhs12" localSheetId="0" hidden="1">integer</definedName>
-    <definedName name="solver_rhs13" localSheetId="0" hidden="1">Challenge3_Day1Submission_jaimi!$B$6</definedName>
-    <definedName name="solver_rhs14" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_rhs15" localSheetId="0" hidden="1">integer</definedName>
-    <definedName name="solver_rhs16" localSheetId="0" hidden="1">Challenge3_Day1Submission_jaimi!$B$7</definedName>
-    <definedName name="solver_rhs17" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_rhs18" localSheetId="0" hidden="1">integer</definedName>
-    <definedName name="solver_rhs19" localSheetId="0" hidden="1">Challenge3_Day1Submission_jaimi!$B$8</definedName>
+    <definedName name="solver_rhs10" localSheetId="0" hidden="1">integer</definedName>
+    <definedName name="solver_rhs11" localSheetId="0" hidden="1">Challenge3_Day1Submission_jaimi!$B$5</definedName>
+    <definedName name="solver_rhs12" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rhs13" localSheetId="0" hidden="1">integer</definedName>
+    <definedName name="solver_rhs14" localSheetId="0" hidden="1">Challenge3_Day1Submission_jaimi!$B$6</definedName>
+    <definedName name="solver_rhs15" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rhs16" localSheetId="0" hidden="1">integer</definedName>
+    <definedName name="solver_rhs17" localSheetId="0" hidden="1">Challenge3_Day1Submission_jaimi!$B$7</definedName>
+    <definedName name="solver_rhs18" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rhs19" localSheetId="0" hidden="1">integer</definedName>
     <definedName name="solver_rhs2" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_rhs20" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_rhs21" localSheetId="0" hidden="1">integer</definedName>
-    <definedName name="solver_rhs22" localSheetId="0" hidden="1">Challenge3_Day1Submission_jaimi!$B$9</definedName>
-    <definedName name="solver_rhs23" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_rhs24" localSheetId="0" hidden="1">integer</definedName>
-    <definedName name="solver_rhs25" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rhs20" localSheetId="0" hidden="1">Challenge3_Day1Submission_jaimi!$B$8</definedName>
+    <definedName name="solver_rhs21" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rhs22" localSheetId="0" hidden="1">integer</definedName>
+    <definedName name="solver_rhs23" localSheetId="0" hidden="1">Challenge3_Day1Submission_jaimi!$B$9</definedName>
+    <definedName name="solver_rhs24" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rhs25" localSheetId="0" hidden="1">integer</definedName>
     <definedName name="solver_rhs26" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rhs27" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rhs28" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rhs29" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rhs3" localSheetId="0" hidden="1">integer</definedName>
-    <definedName name="solver_rhs4" localSheetId="0" hidden="1">Challenge3_Day1Submission_jaimi!$B$3</definedName>
-    <definedName name="solver_rhs5" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_rhs6" localSheetId="0" hidden="1">integer</definedName>
-    <definedName name="solver_rhs7" localSheetId="0" hidden="1">Challenge3_Day1Submission_jaimi!$B$4</definedName>
-    <definedName name="solver_rhs8" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_rhs9" localSheetId="0" hidden="1">integer</definedName>
+    <definedName name="solver_rhs4" localSheetId="0" hidden="1">Challenge3_Day1Submission_jaimi!$T$2:$T$21</definedName>
+    <definedName name="solver_rhs5" localSheetId="0" hidden="1">Challenge3_Day1Submission_jaimi!$B$3</definedName>
+    <definedName name="solver_rhs6" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rhs7" localSheetId="0" hidden="1">integer</definedName>
+    <definedName name="solver_rhs8" localSheetId="0" hidden="1">Challenge3_Day1Submission_jaimi!$B$4</definedName>
+    <definedName name="solver_rhs9" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rlx" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_rsd" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_scl" localSheetId="0" hidden="1">1</definedName>
@@ -132,12 +132,22 @@
     <definedName name="solver_val" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_ver" localSheetId="0" hidden="1">3</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="30">
   <si>
     <t>ID</t>
   </si>
@@ -224,6 +234,9 @@
   </si>
   <si>
     <t>TOTAL PTS (MAXIMIZE THIS)</t>
+  </si>
+  <si>
+    <t>sum_treatments</t>
   </si>
 </sst>
 </file>
@@ -1127,38 +1140,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V24"/>
+  <dimension ref="A1:W24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="U24" sqref="U24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="19.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="19.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="4" style="3" customWidth="1"/>
-    <col min="6" max="6" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="4" style="3" customWidth="1"/>
-    <col min="8" max="8" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="4" style="3" customWidth="1"/>
-    <col min="10" max="10" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="4" style="3" customWidth="1"/>
-    <col min="12" max="12" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.7109375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="4" style="3" customWidth="1"/>
-    <col min="14" max="14" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="4" style="3" customWidth="1"/>
-    <col min="16" max="16" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="4" style="3" customWidth="1"/>
-    <col min="18" max="18" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10.88671875" customWidth="1"/>
-    <col min="20" max="20" width="4" style="3" customWidth="1"/>
-    <col min="21" max="21" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="10.85546875" customWidth="1"/>
+    <col min="21" max="21" width="4" style="3" customWidth="1"/>
+    <col min="22" max="22" width="5.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1216,17 +1229,20 @@
       <c r="S1" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="T1" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="U1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>11</v>
       </c>
-      <c r="V1" s="4" t="s">
+      <c r="W1" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1237,7 +1253,7 @@
         <v>-1</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E2" s="3">
         <v>5</v>
@@ -1285,19 +1301,23 @@
         <f>SUM(F2,P2)</f>
         <v>0</v>
       </c>
-      <c r="T2" s="3">
+      <c r="T2">
+        <f>IF(SUM(F2,H2,J2,L2,N2,P2,R2)&gt;0,1,0)</f>
+        <v>0</v>
+      </c>
+      <c r="U2" s="3">
         <v>10</v>
       </c>
-      <c r="U2">
-        <f>B2+C2+(D2*E2)+(F2*G2)+(H2*I2)+(J2*K2)+(L2*M2)+(N2*O2)+(P2*Q2)+(R2*T2)</f>
-        <v>99</v>
-      </c>
       <c r="V2">
-        <f>IF(U2&gt;100, 100,IF(U2&lt;0,-100,U2))</f>
-        <v>99</v>
-      </c>
-    </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
+        <f>B2+C2+(D2*E2)+(F2*G2)+(H2*I2)+(J2*K2)+(L2*M2)+(N2*O2)+(P2*Q2)+(R2*U2)</f>
+        <v>104</v>
+      </c>
+      <c r="W2">
+        <f>IF(V2&gt;100, 100,IF(V2&lt;0,-100,V2))</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1308,7 +1328,7 @@
         <v>-1</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E3" s="3">
         <v>5</v>
@@ -1356,19 +1376,23 @@
         <f t="shared" ref="S3:S21" si="0">SUM(F3,P3)</f>
         <v>0</v>
       </c>
-      <c r="T3" s="3">
+      <c r="T3">
+        <f t="shared" ref="T3:T21" si="1">IF(SUM(F3,H3,J3,L3,N3,P3,R3)&gt;0,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="U3" s="3">
         <v>10</v>
       </c>
-      <c r="U3">
-        <f t="shared" ref="U3:U21" si="1">B3+C3+(D3*E3)+(F3*G3)+(H3*I3)+(J3*K3)+(L3*M3)+(N3*O3)+(P3*Q3)+(R3*T3)</f>
-        <v>99</v>
-      </c>
       <c r="V3">
-        <f t="shared" ref="V3:V21" si="2">IF(U3&gt;100, 100,IF(U3&lt;0,-100,U3))</f>
-        <v>99</v>
-      </c>
-    </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
+        <f t="shared" ref="V3:V21" si="2">B3+C3+(D3*E3)+(F3*G3)+(H3*I3)+(J3*K3)+(L3*M3)+(N3*O3)+(P3*Q3)+(R3*U3)</f>
+        <v>104</v>
+      </c>
+      <c r="W3">
+        <f t="shared" ref="W3:W21" si="3">IF(V3&gt;100, 100,IF(V3&lt;0,-100,V3))</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1379,7 +1403,7 @@
         <v>-7</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E4" s="3">
         <v>5</v>
@@ -1427,19 +1451,23 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="T4" s="3">
+      <c r="T4">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="U4" s="3">
         <v>10</v>
-      </c>
-      <c r="U4">
-        <f t="shared" si="1"/>
-        <v>98</v>
       </c>
       <c r="V4">
         <f t="shared" si="2"/>
-        <v>98</v>
-      </c>
-    </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+      <c r="W4">
+        <f t="shared" si="3"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1474,7 +1502,7 @@
         <v>15</v>
       </c>
       <c r="L5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M5" s="3">
         <v>30</v>
@@ -1486,7 +1514,7 @@
         <v>25</v>
       </c>
       <c r="P5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q5" s="3">
         <v>15</v>
@@ -1496,21 +1524,25 @@
       </c>
       <c r="S5">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="T5" s="3">
+        <v>0</v>
+      </c>
+      <c r="T5">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="U5" s="3">
         <v>10</v>
-      </c>
-      <c r="U5">
-        <f t="shared" si="1"/>
-        <v>85</v>
       </c>
       <c r="V5">
         <f t="shared" si="2"/>
-        <v>85</v>
-      </c>
-    </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
+        <v>100</v>
+      </c>
+      <c r="W5">
+        <f t="shared" si="3"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1563,25 +1595,29 @@
         <v>15</v>
       </c>
       <c r="R6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S6">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="T6" s="3">
+      <c r="T6">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="U6" s="3">
         <v>10</v>
-      </c>
-      <c r="U6">
-        <f t="shared" si="1"/>
-        <v>93</v>
       </c>
       <c r="V6">
         <f t="shared" si="2"/>
-        <v>93</v>
-      </c>
-    </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+      <c r="W6">
+        <f t="shared" si="3"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1592,7 +1628,7 @@
         <v>-50</v>
       </c>
       <c r="D7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E7" s="3">
         <v>5</v>
@@ -1634,25 +1670,29 @@
         <v>15</v>
       </c>
       <c r="R7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="T7" s="3">
+      <c r="T7">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="U7" s="3">
         <v>10</v>
-      </c>
-      <c r="U7">
-        <f t="shared" si="1"/>
-        <v>104</v>
       </c>
       <c r="V7">
         <f t="shared" si="2"/>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
+        <v>99</v>
+      </c>
+      <c r="W7">
+        <f t="shared" si="3"/>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1663,7 +1703,7 @@
         <v>-60</v>
       </c>
       <c r="D8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E8" s="3">
         <v>5</v>
@@ -1711,19 +1751,23 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="T8" s="3">
+      <c r="T8">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="U8" s="3">
         <v>10</v>
-      </c>
-      <c r="U8">
-        <f t="shared" si="1"/>
-        <v>95</v>
       </c>
       <c r="V8">
         <f t="shared" si="2"/>
-        <v>95</v>
-      </c>
-    </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
+        <v>100</v>
+      </c>
+      <c r="W8">
+        <f t="shared" si="3"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1734,19 +1778,19 @@
         <v>-65</v>
       </c>
       <c r="D9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E9" s="3">
         <v>5</v>
       </c>
       <c r="F9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G9" s="3">
         <v>30</v>
       </c>
       <c r="H9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I9" s="3">
         <v>20</v>
@@ -1758,13 +1802,13 @@
         <v>15</v>
       </c>
       <c r="L9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M9" s="3">
         <v>30</v>
       </c>
       <c r="N9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O9" s="3">
         <v>25</v>
@@ -1776,25 +1820,29 @@
         <v>15</v>
       </c>
       <c r="R9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S9">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="T9" s="3">
+        <v>1</v>
+      </c>
+      <c r="T9">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="U9" s="3">
         <v>10</v>
-      </c>
-      <c r="U9">
-        <f t="shared" si="1"/>
-        <v>-20</v>
       </c>
       <c r="V9">
         <f t="shared" si="2"/>
-        <v>-100</v>
-      </c>
-    </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
+        <v>100</v>
+      </c>
+      <c r="W9">
+        <f t="shared" si="3"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1805,7 +1853,7 @@
         <v>-79</v>
       </c>
       <c r="D10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E10" s="3">
         <v>5</v>
@@ -1847,25 +1895,29 @@
         <v>15</v>
       </c>
       <c r="R10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S10">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="T10" s="3">
+      <c r="T10">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="U10" s="3">
         <v>10</v>
-      </c>
-      <c r="U10">
-        <f t="shared" si="1"/>
-        <v>101</v>
       </c>
       <c r="V10">
         <f t="shared" si="2"/>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
+        <v>96</v>
+      </c>
+      <c r="W10">
+        <f t="shared" si="3"/>
+        <v>96</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1876,7 +1928,7 @@
         <v>-88</v>
       </c>
       <c r="D11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E11" s="3">
         <v>5</v>
@@ -1918,25 +1970,29 @@
         <v>15</v>
       </c>
       <c r="R11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S11">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="T11" s="3">
+      <c r="T11">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="U11" s="3">
         <v>10</v>
-      </c>
-      <c r="U11">
-        <f t="shared" si="1"/>
-        <v>102</v>
       </c>
       <c r="V11">
         <f t="shared" si="2"/>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
+        <v>97</v>
+      </c>
+      <c r="W11">
+        <f t="shared" si="3"/>
+        <v>97</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1947,7 +2003,7 @@
         <v>-62</v>
       </c>
       <c r="D12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E12" s="3">
         <v>5</v>
@@ -1959,7 +2015,7 @@
         <v>30</v>
       </c>
       <c r="H12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I12" s="3">
         <v>20</v>
@@ -1971,43 +2027,47 @@
         <v>15</v>
       </c>
       <c r="L12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M12" s="3">
         <v>30</v>
       </c>
       <c r="N12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O12" s="3">
         <v>25</v>
       </c>
       <c r="P12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q12" s="3">
         <v>15</v>
       </c>
       <c r="R12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S12">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="T12" s="3">
+        <v>1</v>
+      </c>
+      <c r="T12">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="U12" s="3">
         <v>10</v>
-      </c>
-      <c r="U12">
-        <f t="shared" si="1"/>
-        <v>-2</v>
       </c>
       <c r="V12">
         <f t="shared" si="2"/>
-        <v>-100</v>
-      </c>
-    </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+      <c r="W12">
+        <f t="shared" si="3"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2018,7 +2078,7 @@
         <v>-18</v>
       </c>
       <c r="D13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E13" s="3">
         <v>5</v>
@@ -2066,19 +2126,23 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="T13" s="3">
+      <c r="T13">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="U13" s="3">
         <v>10</v>
-      </c>
-      <c r="U13">
-        <f t="shared" si="1"/>
-        <v>109</v>
       </c>
       <c r="V13">
         <f t="shared" si="2"/>
+        <v>114</v>
+      </c>
+      <c r="W13">
+        <f t="shared" si="3"/>
         <v>100</v>
       </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2089,13 +2153,13 @@
         <v>-68</v>
       </c>
       <c r="D14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E14" s="3">
         <v>5</v>
       </c>
       <c r="F14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G14" s="3">
         <v>30</v>
@@ -2107,19 +2171,19 @@
         <v>20</v>
       </c>
       <c r="J14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K14" s="3">
         <v>15</v>
       </c>
       <c r="L14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M14" s="3">
         <v>30</v>
       </c>
       <c r="N14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O14" s="3">
         <v>25</v>
@@ -2131,25 +2195,29 @@
         <v>15</v>
       </c>
       <c r="R14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S14">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="T14" s="3">
+        <v>1</v>
+      </c>
+      <c r="T14">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="U14" s="3">
         <v>10</v>
-      </c>
-      <c r="U14">
-        <f t="shared" si="1"/>
-        <v>-13</v>
       </c>
       <c r="V14">
         <f t="shared" si="2"/>
-        <v>-100</v>
-      </c>
-    </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
+        <v>102</v>
+      </c>
+      <c r="W14">
+        <f t="shared" si="3"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -2208,19 +2276,23 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="T15" s="3">
+      <c r="T15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="U15" s="3">
         <v>10</v>
-      </c>
-      <c r="U15">
-        <f t="shared" si="1"/>
-        <v>-39</v>
       </c>
       <c r="V15">
         <f t="shared" si="2"/>
+        <v>-39</v>
+      </c>
+      <c r="W15">
+        <f t="shared" si="3"/>
         <v>-100</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2279,19 +2351,23 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="T16" s="3">
+      <c r="T16">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="U16" s="3">
         <v>10</v>
-      </c>
-      <c r="U16">
-        <f t="shared" si="1"/>
-        <v>-50</v>
       </c>
       <c r="V16">
         <f t="shared" si="2"/>
+        <v>-50</v>
+      </c>
+      <c r="W16">
+        <f t="shared" si="3"/>
         <v>-100</v>
       </c>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -2302,7 +2378,7 @@
         <v>-13</v>
       </c>
       <c r="D17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E17" s="3">
         <v>5</v>
@@ -2350,19 +2426,23 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="T17" s="3">
+      <c r="T17">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="U17" s="3">
         <v>10</v>
-      </c>
-      <c r="U17">
-        <f t="shared" si="1"/>
-        <v>103</v>
       </c>
       <c r="V17">
         <f t="shared" si="2"/>
+        <v>108</v>
+      </c>
+      <c r="W17">
+        <f t="shared" si="3"/>
         <v>100</v>
       </c>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -2373,7 +2453,7 @@
         <v>-7</v>
       </c>
       <c r="D18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E18" s="3">
         <v>5</v>
@@ -2397,7 +2477,7 @@
         <v>15</v>
       </c>
       <c r="L18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M18" s="3">
         <v>30</v>
@@ -2415,25 +2495,29 @@
         <v>15</v>
       </c>
       <c r="R18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S18">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="T18" s="3">
+      <c r="T18">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="U18" s="3">
         <v>10</v>
-      </c>
-      <c r="U18">
-        <f t="shared" si="1"/>
-        <v>118</v>
       </c>
       <c r="V18">
         <f t="shared" si="2"/>
+        <v>103</v>
+      </c>
+      <c r="W18">
+        <f t="shared" si="3"/>
         <v>100</v>
       </c>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -2444,7 +2528,7 @@
         <v>-1</v>
       </c>
       <c r="D19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E19" s="3">
         <v>5</v>
@@ -2492,19 +2576,23 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="T19" s="3">
+      <c r="T19">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="U19" s="3">
         <v>10</v>
-      </c>
-      <c r="U19">
-        <f t="shared" si="1"/>
-        <v>98</v>
       </c>
       <c r="V19">
         <f t="shared" si="2"/>
-        <v>98</v>
-      </c>
-    </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+      <c r="W19">
+        <f t="shared" si="3"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -2563,19 +2651,23 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="T20" s="3">
+      <c r="T20">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="U20" s="3">
         <v>10</v>
-      </c>
-      <c r="U20">
-        <f t="shared" si="1"/>
-        <v>98</v>
       </c>
       <c r="V20">
         <f t="shared" si="2"/>
         <v>98</v>
       </c>
-    </row>
-    <row r="21" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="W20">
+        <f t="shared" si="3"/>
+        <v>98</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
@@ -2634,19 +2726,23 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="T21" s="3">
+      <c r="T21">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="U21" s="3">
         <v>10</v>
-      </c>
-      <c r="U21">
-        <f t="shared" si="1"/>
-        <v>-60</v>
       </c>
       <c r="V21">
         <f t="shared" si="2"/>
+        <v>-60</v>
+      </c>
+      <c r="W21">
+        <f t="shared" si="3"/>
         <v>-100</v>
       </c>
     </row>
-    <row r="22" spans="1:22" s="2" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:23" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>19</v>
       </c>
@@ -2655,66 +2751,67 @@
         <v>1394</v>
       </c>
       <c r="C22" s="2">
-        <f t="shared" ref="C22:U22" si="3">SUM(C2:C21)</f>
+        <f t="shared" ref="C22:V22" si="4">SUM(C2:C21)</f>
         <v>-836</v>
       </c>
       <c r="D22" s="2">
-        <f t="shared" si="3"/>
-        <v>3</v>
+        <f t="shared" si="4"/>
+        <v>17</v>
       </c>
       <c r="E22" s="3"/>
       <c r="F22" s="2">
-        <f t="shared" si="3"/>
-        <v>2</v>
+        <f t="shared" si="4"/>
+        <v>4</v>
       </c>
       <c r="G22" s="3"/>
       <c r="H22" s="2">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>2</v>
       </c>
       <c r="I22" s="3"/>
       <c r="J22" s="2">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>1</v>
       </c>
       <c r="K22" s="3"/>
       <c r="L22" s="2">
-        <f t="shared" si="3"/>
-        <v>9</v>
+        <f t="shared" si="4"/>
+        <v>12</v>
       </c>
       <c r="M22" s="3"/>
       <c r="N22" s="2">
-        <f t="shared" si="3"/>
-        <v>9</v>
+        <f t="shared" si="4"/>
+        <v>12</v>
       </c>
       <c r="O22" s="3"/>
       <c r="P22" s="2">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="Q22" s="3"/>
       <c r="R22" s="2">
-        <f t="shared" si="3"/>
-        <v>6</v>
+        <f t="shared" si="4"/>
+        <v>8</v>
       </c>
       <c r="S22" s="7"/>
-      <c r="T22" s="3"/>
-      <c r="U22" s="2">
-        <f t="shared" si="3"/>
-        <v>1218</v>
-      </c>
-      <c r="V22" s="5">
-        <f>SUM(V2:V21)</f>
-        <v>765</v>
-      </c>
-    </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="U24" t="s">
+      <c r="T22" s="7"/>
+      <c r="U22" s="3"/>
+      <c r="V22" s="2">
+        <f t="shared" si="4"/>
+        <v>1588</v>
+      </c>
+      <c r="W22" s="5">
+        <f>SUM(W2:W21)</f>
+        <v>1390</v>
+      </c>
+    </row>
+    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="V24" t="s">
         <v>28</v>
       </c>
-      <c r="V24">
-        <f>SUM(V22,bank!G10)</f>
-        <v>1390</v>
+      <c r="W24">
+        <f>SUM(W22,bank!G10)</f>
+        <v>1887.5</v>
       </c>
     </row>
   </sheetData>
@@ -2730,14 +2827,14 @@
       <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="32.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="32.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -2760,7 +2857,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>3</v>
       </c>
@@ -2775,10 +2872,10 @@
       </c>
       <c r="F2">
         <f>B2-Challenge3_Day1Submission_jaimi!D$22</f>
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>4</v>
       </c>
@@ -2796,14 +2893,14 @@
       </c>
       <c r="F3">
         <f>B3-Challenge3_Day1Submission_jaimi!F$22</f>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G3">
         <f t="shared" ref="G3:G9" si="0">(0.5*C3)*F3</f>
-        <v>120</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>5</v>
       </c>
@@ -2821,14 +2918,14 @@
       </c>
       <c r="F4">
         <f>B4-Challenge3_Day1Submission_jaimi!H$22</f>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G4">
         <f t="shared" si="0"/>
-        <v>105</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>6</v>
       </c>
@@ -2843,14 +2940,14 @@
       </c>
       <c r="F5">
         <f>B5-Challenge3_Day1Submission_jaimi!J$22</f>
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G5">
         <f t="shared" si="0"/>
-        <v>250</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+        <v>237.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>7</v>
       </c>
@@ -2865,14 +2962,14 @@
       </c>
       <c r="F6">
         <f>B6-Challenge3_Day1Submission_jaimi!L$22</f>
-        <v>1</v>
+        <v>-2</v>
       </c>
       <c r="G6">
         <f t="shared" si="0"/>
-        <v>7.5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+        <v>-15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>8</v>
       </c>
@@ -2887,14 +2984,14 @@
       </c>
       <c r="F7">
         <f>B7-Challenge3_Day1Submission_jaimi!N$22</f>
-        <v>1</v>
+        <v>-2</v>
       </c>
       <c r="G7">
         <f t="shared" si="0"/>
-        <v>7.5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+        <v>-15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>9</v>
       </c>
@@ -2916,7 +3013,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>10</v>
       </c>
@@ -2931,17 +3028,17 @@
       </c>
       <c r="F9">
         <f>B9-Challenge3_Day1Submission_jaimi!R$22</f>
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G9">
         <f t="shared" si="0"/>
-        <v>55</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G10" s="5">
         <f>SUM(G3:G9)</f>
-        <v>625</v>
+        <v>497.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>